<commit_message>
Ajout d'un script pour changer les graphiques par défaut + ajout de Ecoli avec la modélisation de 100s et 300s
</commit_message>
<xml_diff>
--- a/ecoliModel/init_essais.xlsx
+++ b/ecoliModel/init_essais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Emma\Stage_GB5_LBBE\LBBEModelisation\ecoliModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CF0683-7F76-4BE7-80AA-6B422521BC7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FDE766-78AD-4341-BEEB-3792065A3AB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22572" windowHeight="8484" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="267">
   <si>
     <t>Metabolite</t>
   </si>
@@ -808,10 +808,25 @@
     <t>7.999999999698104</t>
   </si>
   <si>
-    <t>1.2873151241311083</t>
-  </si>
-  <si>
     <t>8.7363521885873</t>
+  </si>
+  <si>
+    <t>0.00010000000001936753</t>
+  </si>
+  <si>
+    <t>2.676318153277067</t>
+  </si>
+  <si>
+    <t>14.008413729564946</t>
+  </si>
+  <si>
+    <t>0.05248431161643879</t>
+  </si>
+  <si>
+    <t>2.7926086603330034</t>
+  </si>
+  <si>
+    <t>1.315108425425397</t>
   </si>
 </sst>
 </file>
@@ -1288,7 +1303,7 @@
   </sheetPr>
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -1437,8 +1452,8 @@
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>261</v>
+      <c r="B18" s="15" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1477,8 +1492,8 @@
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="2">
-        <v>0</v>
+      <c r="B23" s="15" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1493,8 +1508,8 @@
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>260</v>
+      <c r="B25" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1581,8 +1596,8 @@
       <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="15">
-        <v>0</v>
+      <c r="B36" s="15" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1637,8 +1652,8 @@
       <c r="A43" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="2">
-        <v>0</v>
+      <c r="B43" s="15" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1653,8 +1668,8 @@
       <c r="A45" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B45" s="2">
-        <v>0</v>
+      <c r="B45" s="15" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1685,8 +1700,8 @@
       <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B49" s="2">
-        <v>0</v>
+      <c r="B49" s="15" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1717,8 +1732,8 @@
       <c r="A53" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B53" s="2">
-        <v>0</v>
+      <c r="B53" s="15" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>